<commit_message>
lectura con datos dezplazados
</commit_message>
<xml_diff>
--- a/control_reparaciones/dataframe/data.xlsx
+++ b/control_reparaciones/dataframe/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documentos\Workspace\workspace-python\control_reparaciones\dataframe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D98649-2C54-4946-AAC2-66E132DD90FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2133A584-35F1-49B7-BF49-8ADCD0CB11A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -360,82 +360,84 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="B4:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B5">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="C5">
         <v>5</v>
       </c>
-      <c r="C2">
+      <c r="D5">
         <v>3.5</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B6">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="C6">
         <v>10.199999999999999</v>
       </c>
-      <c r="C3">
+      <c r="D6">
         <v>7.8</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B7">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="C7">
         <v>4.5</v>
       </c>
-      <c r="C4">
+      <c r="D7">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B8">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="C8">
         <v>12</v>
       </c>
-      <c r="C5">
+      <c r="D8">
         <v>6.5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B9">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="C9">
         <v>8.6999999999999993</v>
       </c>
-      <c r="C6">
+      <c r="D9">
         <v>9.1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="H12" s="1"/>
+      <c r="N12" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>